<commit_message>
Add units to SGMS Rev D CPL
</commit_message>
<xml_diff>
--- a/Diptrace/Gerber/SGMS REVD Support Files/SGMS RevD CPL.xlsx
+++ b/Diptrace/Gerber/SGMS REVD Support Files/SGMS RevD CPL.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brenn\Desktop\Baja\Github\not-code\Diptrace\Gerber\SGMS REVD Support Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\techw\Documents\Baja SAE\GitHub\not-code\Diptrace\Gerber\SGMS REVD Support Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F68FD4C-5BA9-4989-9B4E-5A0282C343E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E84D345-32C5-484C-A103-626D4B591BE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1020" yWindow="-120" windowWidth="27900" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="14">
   <si>
     <t>Designator</t>
   </si>
@@ -41,6 +41,27 @@
   </si>
   <si>
     <t>TS972IDT</t>
+  </si>
+  <si>
+    <t>22.427mm</t>
+  </si>
+  <si>
+    <t>22.225mm</t>
+  </si>
+  <si>
+    <t>74.295mm</t>
+  </si>
+  <si>
+    <t>42.07mm</t>
+  </si>
+  <si>
+    <t>31.275mm</t>
+  </si>
+  <si>
+    <t>20.48mm</t>
+  </si>
+  <si>
+    <t>9.685mm</t>
   </si>
 </sst>
 </file>
@@ -392,16 +413,16 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" customWidth="1"/>
-    <col min="2" max="2" width="16.1796875" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -425,11 +446,11 @@
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2">
-        <v>22.427</v>
-      </c>
-      <c r="C2" s="2">
-        <v>42.07</v>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>5</v>
@@ -442,11 +463,11 @@
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2">
-        <v>22.225000000000001</v>
-      </c>
-      <c r="C3" s="2">
-        <v>31.274999999999999</v>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>5</v>
@@ -459,11 +480,11 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
-        <v>22.225000000000001</v>
-      </c>
-      <c r="C4" s="2">
-        <v>20.48</v>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>5</v>
@@ -476,11 +497,11 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
-        <v>22.225000000000001</v>
-      </c>
-      <c r="C5" s="2">
-        <v>9.6850000000000005</v>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>5</v>
@@ -493,11 +514,11 @@
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="2">
-        <v>74.295000000000002</v>
-      </c>
-      <c r="C6" s="2">
-        <v>42.07</v>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>5</v>
@@ -510,11 +531,11 @@
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="2">
-        <v>74.295000000000002</v>
-      </c>
-      <c r="C7" s="2">
-        <v>31.274999999999999</v>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>5</v>
@@ -527,11 +548,11 @@
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2">
-        <v>74.295000000000002</v>
-      </c>
-      <c r="C8" s="2">
-        <v>20.48</v>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>5</v>
@@ -544,11 +565,11 @@
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2">
-        <v>74.295000000000002</v>
-      </c>
-      <c r="C9" s="2">
-        <v>9.6850000000000005</v>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>5</v>

</xml_diff>